<commit_message>
Fix surgut (aspect > sibir), add vlg-auto34
</commit_message>
<xml_diff>
--- a/xlsx/chelyabinsk.xlsx
+++ b/xlsx/chelyabinsk.xlsx
@@ -654,7 +654,7 @@
         </is>
       </c>
       <c r="V3" t="n">
-        <v>1248000</v>
+        <v>1133000</v>
       </c>
       <c r="W3" t="inlineStr">
         <is>
@@ -758,7 +758,7 @@
         </is>
       </c>
       <c r="V5" t="n">
-        <v>1335000</v>
+        <v>1013000</v>
       </c>
       <c r="W5" t="inlineStr">
         <is>
@@ -821,7 +821,7 @@
         </is>
       </c>
       <c r="V6" t="n">
-        <v>1782000</v>
+        <v>1770000</v>
       </c>
       <c r="W6" t="inlineStr">
         <is>
@@ -922,7 +922,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>1383594</v>
+        <v>805900</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -930,7 +930,7 @@
         </is>
       </c>
       <c r="V9" t="n">
-        <v>1383594</v>
+        <v>805900</v>
       </c>
       <c r="W9" t="inlineStr">
         <is>
@@ -991,7 +991,7 @@
         </is>
       </c>
       <c r="V10" t="n">
-        <v>1098000</v>
+        <v>574000</v>
       </c>
       <c r="W10" t="inlineStr">
         <is>
@@ -1177,7 +1177,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>https://kc-klassavto.ru/auto/changan/cs55/</t>
+          <t>https://carsklad-174.ru/auto/changan/cs55/i/suv-5d</t>
         </is>
       </c>
       <c r="F14" t="n">
@@ -1217,7 +1217,7 @@
         </is>
       </c>
       <c r="V14" t="n">
-        <v>999000</v>
+        <v>759900</v>
       </c>
       <c r="W14" t="inlineStr">
         <is>
@@ -1296,7 +1296,7 @@
         </is>
       </c>
       <c r="V15" t="n">
-        <v>1238900</v>
+        <v>1233900</v>
       </c>
       <c r="W15" t="inlineStr">
         <is>
@@ -1408,7 +1408,7 @@
         </is>
       </c>
       <c r="V17" t="n">
-        <v>1089300</v>
+        <v>1084300</v>
       </c>
       <c r="W17" t="inlineStr">
         <is>
@@ -1479,7 +1479,7 @@
         </is>
       </c>
       <c r="V18" t="n">
-        <v>2225940</v>
+        <v>2079900</v>
       </c>
       <c r="W18" t="inlineStr">
         <is>
@@ -1646,7 +1646,7 @@
         </is>
       </c>
       <c r="V21" t="n">
-        <v>1451940</v>
+        <v>1319900</v>
       </c>
       <c r="W21" t="inlineStr">
         <is>
@@ -1781,7 +1781,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>https://kc-klassavto.ru/auto/changan/uni-k/</t>
+          <t>https://carsklad-174.ru/auto/changan/uni-k/i/suv-5d</t>
         </is>
       </c>
       <c r="F24" t="n">
@@ -1821,7 +1821,7 @@
         </is>
       </c>
       <c r="V24" t="n">
-        <v>2068900</v>
+        <v>2039900</v>
       </c>
       <c r="W24" t="inlineStr">
         <is>
@@ -1992,7 +1992,7 @@
         </is>
       </c>
       <c r="V27" t="n">
-        <v>1628900</v>
+        <v>1623900</v>
       </c>
       <c r="W27" t="inlineStr">
         <is>
@@ -2185,7 +2185,7 @@
         </is>
       </c>
       <c r="V30" t="n">
-        <v>565900</v>
+        <v>560900</v>
       </c>
       <c r="W30" t="inlineStr">
         <is>
@@ -2450,7 +2450,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>https://avto-graf-newcars.ru/catalog/chery/tiggo7pro</t>
+          <t>https://carsklad-174.ru/auto/chery/tiggo-7-pro/i/suv-5d</t>
         </is>
       </c>
       <c r="F35" t="n">
@@ -2490,7 +2490,7 @@
         </is>
       </c>
       <c r="V35" t="n">
-        <v>1108900</v>
+        <v>1087900</v>
       </c>
       <c r="W35" t="inlineStr">
         <is>
@@ -2569,7 +2569,7 @@
         </is>
       </c>
       <c r="V36" t="n">
-        <v>1304000</v>
+        <v>1299000</v>
       </c>
       <c r="W36" t="inlineStr">
         <is>
@@ -2755,7 +2755,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>https://avto-graf-newcars.ru/catalog/chery/tiggo_8_pro</t>
+          <t>https://carsklad-174.ru/auto/chery/tiggo-8-pro/i/suv-5d</t>
         </is>
       </c>
       <c r="F40" t="n">
@@ -2795,7 +2795,7 @@
         </is>
       </c>
       <c r="V40" t="n">
-        <v>1778900</v>
+        <v>1179900</v>
       </c>
       <c r="W40" t="inlineStr">
         <is>
@@ -2901,7 +2901,7 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>1980000</v>
+        <v>1549900</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -2929,7 +2929,7 @@
         </is>
       </c>
       <c r="V42" t="n">
-        <v>1980000</v>
+        <v>1549900</v>
       </c>
       <c r="W42" t="inlineStr">
         <is>
@@ -3074,7 +3074,7 @@
         </is>
       </c>
       <c r="V45" t="n">
-        <v>542900</v>
+        <v>537900</v>
       </c>
       <c r="W45" t="inlineStr">
         <is>
@@ -3153,7 +3153,7 @@
         </is>
       </c>
       <c r="V46" t="n">
-        <v>492900</v>
+        <v>487900</v>
       </c>
       <c r="W46" t="inlineStr">
         <is>
@@ -3232,7 +3232,7 @@
         </is>
       </c>
       <c r="V47" t="n">
-        <v>542900</v>
+        <v>537900</v>
       </c>
       <c r="W47" t="inlineStr">
         <is>
@@ -3463,11 +3463,11 @@
         </is>
       </c>
       <c r="D52" t="n">
-        <v>759000</v>
+        <v>754000</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>https://che-motors-2024.ru/catalog/dongfeng/580</t>
+          <t>https://carsklad-174.ru/auto/dfm/580/ii/suv-5d</t>
         </is>
       </c>
       <c r="F52" t="n">
@@ -3487,7 +3487,7 @@
         </is>
       </c>
       <c r="V52" t="n">
-        <v>1499400</v>
+        <v>754000</v>
       </c>
       <c r="W52" t="inlineStr">
         <is>
@@ -3699,7 +3699,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>https://avto-graf-newcars.ru/catalog/exeed/txl</t>
+          <t>https://carsklad-174.ru/auto/exeed/txl/i/suv-5d</t>
         </is>
       </c>
       <c r="F56" t="n">
@@ -3739,7 +3739,7 @@
         </is>
       </c>
       <c r="V56" t="n">
-        <v>1832900</v>
+        <v>1399900</v>
       </c>
       <c r="W56" t="inlineStr">
         <is>
@@ -4201,7 +4201,7 @@
         </is>
       </c>
       <c r="V64" t="n">
-        <v>961200</v>
+        <v>614300</v>
       </c>
       <c r="W64" t="inlineStr">
         <is>
@@ -4264,7 +4264,7 @@
         </is>
       </c>
       <c r="V65" t="n">
-        <v>904800</v>
+        <v>756000</v>
       </c>
       <c r="W65" t="inlineStr">
         <is>
@@ -4630,7 +4630,7 @@
         </is>
       </c>
       <c r="V71" t="n">
-        <v>869900</v>
+        <v>864900</v>
       </c>
       <c r="W71" t="inlineStr">
         <is>
@@ -4669,31 +4669,31 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
+          <t>https://carsklad-174.ru/auto/geely/atlas/ii/suv-5d</t>
+        </is>
+      </c>
+      <c r="R72" t="inlineStr">
+        <is>
+          <t>2236493</t>
+        </is>
+      </c>
+      <c r="S72" t="inlineStr">
+        <is>
+          <t>https://ac-174auto.ru/auto/geely/atlas/</t>
+        </is>
+      </c>
+      <c r="T72" t="inlineStr">
+        <is>
+          <t>1529000</t>
+        </is>
+      </c>
+      <c r="U72" t="inlineStr">
+        <is>
           <t>https://kc-klassavto.ru/auto/geely/atlas/</t>
         </is>
       </c>
-      <c r="R72" t="inlineStr">
-        <is>
-          <t>2236493</t>
-        </is>
-      </c>
-      <c r="S72" t="inlineStr">
-        <is>
-          <t>https://ac-174auto.ru/auto/geely/atlas/</t>
-        </is>
-      </c>
-      <c r="T72" t="inlineStr">
-        <is>
-          <t>1529000</t>
-        </is>
-      </c>
-      <c r="U72" t="inlineStr">
-        <is>
-          <t>https://kc-klassavto.ru/auto/geely/atlas/</t>
-        </is>
-      </c>
       <c r="V72" t="n">
-        <v>2054514</v>
+        <v>1529000</v>
       </c>
       <c r="W72" t="inlineStr">
         <is>
@@ -4772,7 +4772,7 @@
         </is>
       </c>
       <c r="V73" t="n">
-        <v>1087596</v>
+        <v>1082596</v>
       </c>
       <c r="W73" t="inlineStr">
         <is>
@@ -4866,7 +4866,7 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>https://kc-klassavto.ru/auto/geely/coolray_1/</t>
+          <t>https://carsklad-174.ru/auto/geely/coolray/i/suv-5d</t>
         </is>
       </c>
       <c r="F75" t="n">
@@ -4906,7 +4906,7 @@
         </is>
       </c>
       <c r="V75" t="n">
-        <v>1196994</v>
+        <v>619990</v>
       </c>
       <c r="W75" t="inlineStr">
         <is>
@@ -4945,31 +4945,31 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
+          <t>https://carsklad-174.ru/auto/geely/coolray/i-restyling/suv-5d</t>
+        </is>
+      </c>
+      <c r="R76" t="inlineStr">
+        <is>
+          <t>1244900</t>
+        </is>
+      </c>
+      <c r="S76" t="inlineStr">
+        <is>
+          <t>https://ac-174auto.ru/auto/geely/coolray/</t>
+        </is>
+      </c>
+      <c r="T76" t="inlineStr">
+        <is>
+          <t>1219990</t>
+        </is>
+      </c>
+      <c r="U76" t="inlineStr">
+        <is>
           <t>https://kc-klassavto.ru/auto/geely/coolray/</t>
         </is>
       </c>
-      <c r="R76" t="inlineStr">
-        <is>
-          <t>1244900</t>
-        </is>
-      </c>
-      <c r="S76" t="inlineStr">
-        <is>
-          <t>https://ac-174auto.ru/auto/geely/coolray/</t>
-        </is>
-      </c>
-      <c r="T76" t="inlineStr">
-        <is>
-          <t>1219990</t>
-        </is>
-      </c>
-      <c r="U76" t="inlineStr">
-        <is>
-          <t>https://kc-klassavto.ru/auto/geely/coolray/</t>
-        </is>
-      </c>
       <c r="V76" t="n">
-        <v>1627914</v>
+        <v>1219990</v>
       </c>
       <c r="W76" t="inlineStr">
         <is>
@@ -5238,7 +5238,7 @@
         </is>
       </c>
       <c r="V81" t="n">
-        <v>2694114</v>
+        <v>2689900</v>
       </c>
       <c r="W81" t="inlineStr">
         <is>
@@ -5345,7 +5345,7 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>https://avto-graf-newcars.ru/catalog/geely/tugella</t>
+          <t>https://carsklad-174.ru/auto/geely/tugella/i-restyling/suv-5d</t>
         </is>
       </c>
       <c r="F84" t="n">
@@ -5357,7 +5357,7 @@
         </is>
       </c>
       <c r="V84" t="n">
-        <v>2375994</v>
+        <v>1859990</v>
       </c>
       <c r="W84" t="inlineStr">
         <is>
@@ -5580,7 +5580,7 @@
         </is>
       </c>
       <c r="V89" t="n">
-        <v>1679000</v>
+        <v>1674000</v>
       </c>
       <c r="W89" t="inlineStr">
         <is>
@@ -5619,7 +5619,7 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>https://kc-klassavto.ru/auto/haval/dargo_x/</t>
+          <t>https://carsklad-174.ru/auto/haval/dargo/i/x</t>
         </is>
       </c>
       <c r="F90" t="n">
@@ -5641,7 +5641,7 @@
         </is>
       </c>
       <c r="V90" t="n">
-        <v>2009400</v>
+        <v>1959000</v>
       </c>
       <c r="W90" t="inlineStr">
         <is>
@@ -5670,7 +5670,7 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>https://avto-graf-newcars.ru/catalog/haval/f7</t>
+          <t>https://carsklad-174.ru/auto/haval/f_7/i/suv-5d</t>
         </is>
       </c>
       <c r="F91" t="n">
@@ -5690,7 +5690,7 @@
         </is>
       </c>
       <c r="V91" t="n">
-        <v>1469400</v>
+        <v>1119000</v>
       </c>
       <c r="W91" t="inlineStr">
         <is>
@@ -5774,7 +5774,7 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>https://avto-graf-newcars.ru/catalog/haval/f7x</t>
+          <t>https://carsklad-174.ru/auto/haval/f_7_x/i/suv-5d</t>
         </is>
       </c>
       <c r="F93" t="n">
@@ -5794,7 +5794,7 @@
         </is>
       </c>
       <c r="V93" t="n">
-        <v>1499400</v>
+        <v>1199000</v>
       </c>
       <c r="W93" t="inlineStr">
         <is>
@@ -6088,7 +6088,7 @@
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>https://avto-graf-newcars.ru/catalog/haval/h9_2018</t>
+          <t>https://carsklad-174.ru/auto/haval/h9/i/suv-5d</t>
         </is>
       </c>
       <c r="F99" t="n">
@@ -6118,7 +6118,7 @@
         </is>
       </c>
       <c r="V99" t="n">
-        <v>1909300</v>
+        <v>1803000</v>
       </c>
       <c r="W99" t="inlineStr">
         <is>
@@ -6190,7 +6190,7 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>https://kc-klassavto.ru/auto/haval/jolion_1/</t>
+          <t>https://carsklad-174.ru/auto/haval/jolion/i/suv-5d</t>
         </is>
       </c>
       <c r="F101" t="n">
@@ -6230,7 +6230,7 @@
         </is>
       </c>
       <c r="V101" t="n">
-        <v>1169400</v>
+        <v>689900</v>
       </c>
       <c r="W101" t="inlineStr">
         <is>
@@ -6269,31 +6269,31 @@
       </c>
       <c r="E102" t="inlineStr">
         <is>
+          <t>https://carsklad-174.ru/auto/haval/jolion/i-rest/suv-5d</t>
+        </is>
+      </c>
+      <c r="R102" t="inlineStr">
+        <is>
+          <t>1399300</t>
+        </is>
+      </c>
+      <c r="S102" t="inlineStr">
+        <is>
+          <t>https://ac-174auto.ru/auto/haval/jolion/</t>
+        </is>
+      </c>
+      <c r="T102" t="inlineStr">
+        <is>
+          <t>1199000</t>
+        </is>
+      </c>
+      <c r="U102" t="inlineStr">
+        <is>
           <t>https://kc-klassavto.ru/auto/haval/jolion/</t>
         </is>
       </c>
-      <c r="R102" t="inlineStr">
-        <is>
-          <t>1399300</t>
-        </is>
-      </c>
-      <c r="S102" t="inlineStr">
-        <is>
-          <t>https://ac-174auto.ru/auto/haval/jolion/</t>
-        </is>
-      </c>
-      <c r="T102" t="inlineStr">
-        <is>
-          <t>1199000</t>
-        </is>
-      </c>
-      <c r="U102" t="inlineStr">
-        <is>
-          <t>https://kc-klassavto.ru/auto/haval/jolion/</t>
-        </is>
-      </c>
       <c r="V102" t="n">
-        <v>1199400</v>
+        <v>1199000</v>
       </c>
       <c r="W102" t="inlineStr">
         <is>
@@ -6425,7 +6425,7 @@
         </is>
       </c>
       <c r="V104" t="n">
-        <v>676000</v>
+        <v>671000</v>
       </c>
       <c r="W104" t="inlineStr">
         <is>
@@ -6529,7 +6529,7 @@
         </is>
       </c>
       <c r="V106" t="n">
-        <v>868000</v>
+        <v>863000</v>
       </c>
       <c r="W106" t="inlineStr">
         <is>
@@ -6717,7 +6717,7 @@
         </is>
       </c>
       <c r="V110" t="n">
-        <v>465000</v>
+        <v>460000</v>
       </c>
       <c r="W110" t="inlineStr">
         <is>
@@ -6756,7 +6756,7 @@
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>https://avto-graf-newcars.ru/catalog/hyundai/sonata_2019</t>
+          <t>https://carsklad-174.ru/auto/hyundai/sonata/viii/sedan</t>
         </is>
       </c>
       <c r="F111" t="n">
@@ -6796,7 +6796,7 @@
         </is>
       </c>
       <c r="V111" t="n">
-        <v>1661400</v>
+        <v>1432000</v>
       </c>
       <c r="W111" t="inlineStr">
         <is>
@@ -6868,7 +6868,7 @@
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>https://avto-graf-newcars.ru/catalog/hyundai/tucson_21</t>
+          <t>https://carsklad-174.ru/auto/hyundai/tucson/iv/suv-5d</t>
         </is>
       </c>
       <c r="F113" t="n">
@@ -6898,7 +6898,7 @@
         </is>
       </c>
       <c r="V113" t="n">
-        <v>1478000</v>
+        <v>1429000</v>
       </c>
       <c r="W113" t="inlineStr">
         <is>
@@ -7005,7 +7005,7 @@
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>https://avto-graf-newcars.ru/catalog/jac/j7</t>
+          <t>https://carsklad-174.ru/auto/jac/j7/i/liftback</t>
         </is>
       </c>
       <c r="F116" t="n">
@@ -7045,7 +7045,7 @@
         </is>
       </c>
       <c r="V116" t="n">
-        <v>718000</v>
+        <v>709000</v>
       </c>
       <c r="W116" t="inlineStr">
         <is>
@@ -7890,7 +7890,7 @@
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>https://avto-graf-newcars.ru/catalog/jetta/va3</t>
+          <t>https://carsklad-174.ru/auto/jetta/va3/i/sedan</t>
         </is>
       </c>
       <c r="F133" t="n">
@@ -7922,7 +7922,7 @@
         </is>
       </c>
       <c r="V133" t="n">
-        <v>1014000</v>
+        <v>840000</v>
       </c>
       <c r="W133" t="inlineStr">
         <is>
@@ -7961,7 +7961,7 @@
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>https://avto-graf-newcars.ru/catalog/jetta/vs5</t>
+          <t>https://carsklad-174.ru/auto/jetta/vs5/i/suv-5d</t>
         </is>
       </c>
       <c r="F134" t="n">
@@ -7993,7 +7993,7 @@
         </is>
       </c>
       <c r="V134" t="n">
-        <v>1194000</v>
+        <v>1140000</v>
       </c>
       <c r="W134" t="inlineStr">
         <is>
@@ -8127,7 +8127,7 @@
         </is>
       </c>
       <c r="V136" t="n">
-        <v>1269000</v>
+        <v>1053000</v>
       </c>
       <c r="W136" t="inlineStr">
         <is>
@@ -8190,7 +8190,7 @@
         </is>
       </c>
       <c r="V137" t="n">
-        <v>1342800</v>
+        <v>1317900</v>
       </c>
       <c r="W137" t="inlineStr">
         <is>
@@ -8253,7 +8253,7 @@
         </is>
       </c>
       <c r="V138" t="n">
-        <v>1508940</v>
+        <v>1350000</v>
       </c>
       <c r="W138" t="inlineStr">
         <is>
@@ -8420,7 +8420,7 @@
         </is>
       </c>
       <c r="V141" t="n">
-        <v>1346940</v>
+        <v>859900</v>
       </c>
       <c r="W141" t="inlineStr">
         <is>
@@ -8491,7 +8491,7 @@
         </is>
       </c>
       <c r="V142" t="n">
-        <v>1388940</v>
+        <v>969900</v>
       </c>
       <c r="W142" t="inlineStr">
         <is>
@@ -8562,7 +8562,7 @@
         </is>
       </c>
       <c r="V143" t="n">
-        <v>1295940</v>
+        <v>943990</v>
       </c>
       <c r="W143" t="inlineStr">
         <is>
@@ -8633,7 +8633,7 @@
         </is>
       </c>
       <c r="V144" t="n">
-        <v>1640940</v>
+        <v>1065300</v>
       </c>
       <c r="W144" t="inlineStr">
         <is>
@@ -8738,7 +8738,7 @@
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>https://kc-klassavto.ru/auto/kia/picanto/</t>
+          <t>https://carsklad-174.ru/auto/kia/picanto/iii-restyling/hatchback-5d</t>
         </is>
       </c>
       <c r="F147" t="n">
@@ -8770,7 +8770,7 @@
         </is>
       </c>
       <c r="V147" t="n">
-        <v>800940</v>
+        <v>619900</v>
       </c>
       <c r="W147" t="inlineStr">
         <is>
@@ -8904,7 +8904,7 @@
         </is>
       </c>
       <c r="V149" t="n">
-        <v>860940</v>
+        <v>460900</v>
       </c>
       <c r="W149" t="inlineStr">
         <is>
@@ -8975,7 +8975,7 @@
         </is>
       </c>
       <c r="V150" t="n">
-        <v>944940</v>
+        <v>590900</v>
       </c>
       <c r="W150" t="inlineStr">
         <is>
@@ -9089,7 +9089,7 @@
         </is>
       </c>
       <c r="V152" t="n">
-        <v>1238940</v>
+        <v>920300</v>
       </c>
       <c r="W152" t="inlineStr">
         <is>
@@ -9193,7 +9193,7 @@
         </is>
       </c>
       <c r="V154" t="n">
-        <v>1160940</v>
+        <v>571200</v>
       </c>
       <c r="W154" t="inlineStr">
         <is>
@@ -9391,7 +9391,7 @@
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>https://avto-graf-newcars.ru/catalog/lada/granta_cross_2019</t>
+          <t>https://carsklad-174.ru/auto/lada/granta/i-restyling/cross</t>
         </is>
       </c>
       <c r="F158" t="n">
@@ -9431,7 +9431,7 @@
         </is>
       </c>
       <c r="V158" t="n">
-        <v>425900</v>
+        <v>304400</v>
       </c>
       <c r="W158" t="inlineStr">
         <is>
@@ -9510,7 +9510,7 @@
         </is>
       </c>
       <c r="V159" t="n">
-        <v>268500</v>
+        <v>263500</v>
       </c>
       <c r="W159" t="inlineStr">
         <is>
@@ -9589,7 +9589,7 @@
         </is>
       </c>
       <c r="V160" t="n">
-        <v>272300</v>
+        <v>267300</v>
       </c>
       <c r="W160" t="inlineStr">
         <is>
@@ -9668,7 +9668,7 @@
         </is>
       </c>
       <c r="V161" t="n">
-        <v>257900</v>
+        <v>252900</v>
       </c>
       <c r="W161" t="inlineStr">
         <is>
@@ -9707,7 +9707,7 @@
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>https://avto-graf-newcars.ru/catalog/lada/granta_da</t>
+          <t>https://carsklad-174.ru/auto/lada/granta/i-restyling/drive-active</t>
         </is>
       </c>
       <c r="F162" t="n">
@@ -9747,7 +9747,7 @@
         </is>
       </c>
       <c r="V162" t="n">
-        <v>425900</v>
+        <v>412500</v>
       </c>
       <c r="W162" t="inlineStr">
         <is>
@@ -9958,7 +9958,7 @@
         </is>
       </c>
       <c r="V167" t="n">
-        <v>278900</v>
+        <v>273900</v>
       </c>
       <c r="W167" t="inlineStr">
         <is>
@@ -10027,7 +10027,7 @@
         </is>
       </c>
       <c r="V168" t="n">
-        <v>348900</v>
+        <v>343900</v>
       </c>
       <c r="W168" t="inlineStr">
         <is>
@@ -10096,7 +10096,7 @@
         </is>
       </c>
       <c r="V169" t="n">
-        <v>384300</v>
+        <v>379300</v>
       </c>
       <c r="W169" t="inlineStr">
         <is>
@@ -10554,7 +10554,7 @@
         </is>
       </c>
       <c r="V179" t="n">
-        <v>360200</v>
+        <v>355200</v>
       </c>
       <c r="W179" t="inlineStr">
         <is>
@@ -10633,7 +10633,7 @@
         </is>
       </c>
       <c r="V180" t="n">
-        <v>444500</v>
+        <v>439500</v>
       </c>
       <c r="W180" t="inlineStr">
         <is>
@@ -10767,7 +10767,7 @@
         </is>
       </c>
       <c r="V182" t="n">
-        <v>433000</v>
+        <v>428000</v>
       </c>
       <c r="W182" t="inlineStr">
         <is>
@@ -10846,7 +10846,7 @@
         </is>
       </c>
       <c r="V183" t="n">
-        <v>1127400</v>
+        <v>585900</v>
       </c>
       <c r="W183" t="inlineStr">
         <is>
@@ -11068,7 +11068,7 @@
         </is>
       </c>
       <c r="V187" t="n">
-        <v>380900</v>
+        <v>375900</v>
       </c>
       <c r="W187" t="inlineStr">
         <is>
@@ -11147,7 +11147,7 @@
         </is>
       </c>
       <c r="V188" t="n">
-        <v>465900</v>
+        <v>460900</v>
       </c>
       <c r="W188" t="inlineStr">
         <is>
@@ -11367,7 +11367,7 @@
         </is>
       </c>
       <c r="V192" t="n">
-        <v>385900</v>
+        <v>380900</v>
       </c>
       <c r="W192" t="inlineStr">
         <is>
@@ -11446,7 +11446,7 @@
         </is>
       </c>
       <c r="V193" t="n">
-        <v>384300</v>
+        <v>379300</v>
       </c>
       <c r="W193" t="inlineStr">
         <is>
@@ -12162,7 +12162,7 @@
         </is>
       </c>
       <c r="V207" t="n">
-        <v>2460000</v>
+        <v>2434000</v>
       </c>
       <c r="W207" t="inlineStr">
         <is>
@@ -12242,7 +12242,7 @@
       </c>
       <c r="E209" t="inlineStr">
         <is>
-          <t>https://kc-klassavto.ru/auto/nissan/qashqai/</t>
+          <t>https://carsklad-174.ru/auto/nissan/qashqai/2-rest/suv-5d</t>
         </is>
       </c>
       <c r="F209" t="n">
@@ -12282,7 +12282,7 @@
         </is>
       </c>
       <c r="V209" t="n">
-        <v>897000</v>
+        <v>880000</v>
       </c>
       <c r="W209" t="inlineStr">
         <is>
@@ -12321,7 +12321,7 @@
       </c>
       <c r="E210" t="inlineStr">
         <is>
-          <t>https://kc-klassavto.ru/auto/nissan/terrano/</t>
+          <t>https://carsklad-174.ru/auto/nissan/terrano/iii/suv-5d</t>
         </is>
       </c>
       <c r="F210" t="n">
@@ -12361,7 +12361,7 @@
         </is>
       </c>
       <c r="V210" t="n">
-        <v>638000</v>
+        <v>619000</v>
       </c>
       <c r="W210" t="inlineStr">
         <is>
@@ -12440,7 +12440,7 @@
         </is>
       </c>
       <c r="V211" t="n">
-        <v>1134000</v>
+        <v>1129000</v>
       </c>
       <c r="W211" t="inlineStr">
         <is>
@@ -12519,7 +12519,7 @@
         </is>
       </c>
       <c r="V212" t="n">
-        <v>1268900</v>
+        <v>1263900</v>
       </c>
       <c r="W212" t="inlineStr">
         <is>
@@ -12822,7 +12822,7 @@
         </is>
       </c>
       <c r="V217" t="n">
-        <v>858000</v>
+        <v>853000</v>
       </c>
       <c r="W217" t="inlineStr">
         <is>
@@ -12891,7 +12891,7 @@
         </is>
       </c>
       <c r="V218" t="n">
-        <v>475000</v>
+        <v>470000</v>
       </c>
       <c r="W218" t="inlineStr">
         <is>
@@ -12965,7 +12965,7 @@
       </c>
       <c r="E220" t="inlineStr">
         <is>
-          <t>https://avto-graf-newcars.ru/catalog/renault/kaptur_2020</t>
+          <t>https://carsklad-174.ru/auto/renault/kaptur/i-rest/suv-5d</t>
         </is>
       </c>
       <c r="F220" t="n">
@@ -13005,7 +13005,7 @@
         </is>
       </c>
       <c r="V220" t="n">
-        <v>713000</v>
+        <v>614000</v>
       </c>
       <c r="W220" t="inlineStr">
         <is>
@@ -13119,7 +13119,7 @@
         </is>
       </c>
       <c r="V222" t="n">
-        <v>395000</v>
+        <v>390000</v>
       </c>
       <c r="W222" t="inlineStr">
         <is>
@@ -13198,7 +13198,7 @@
         </is>
       </c>
       <c r="V223" t="n">
-        <v>503990</v>
+        <v>498990</v>
       </c>
       <c r="W223" t="inlineStr">
         <is>
@@ -13348,7 +13348,7 @@
         </is>
       </c>
       <c r="V225" t="n">
-        <v>395000</v>
+        <v>390000</v>
       </c>
       <c r="W225" t="inlineStr">
         <is>
@@ -13427,7 +13427,7 @@
         </is>
       </c>
       <c r="V226" t="n">
-        <v>399000</v>
+        <v>394000</v>
       </c>
       <c r="W226" t="inlineStr">
         <is>
@@ -13557,7 +13557,7 @@
         </is>
       </c>
       <c r="V228" t="n">
-        <v>954000</v>
+        <v>949000</v>
       </c>
       <c r="W228" t="inlineStr">
         <is>
@@ -13708,31 +13708,31 @@
       </c>
       <c r="E231" t="inlineStr">
         <is>
+          <t>https://carsklad-174.ru/auto/skoda/kodiaq/i-rest/laurin</t>
+        </is>
+      </c>
+      <c r="R231" t="inlineStr">
+        <is>
+          <t>3483600</t>
+        </is>
+      </c>
+      <c r="S231" t="inlineStr">
+        <is>
+          <t>https://ac-174auto.ru/auto/skoda/kodiaq_laurin__klement/</t>
+        </is>
+      </c>
+      <c r="T231" t="inlineStr">
+        <is>
+          <t>3058000</t>
+        </is>
+      </c>
+      <c r="U231" t="inlineStr">
+        <is>
           <t>https://kc-klassavto.ru/auto/skoda/kodiaq_laurin__klement/</t>
         </is>
       </c>
-      <c r="R231" t="inlineStr">
-        <is>
-          <t>3483600</t>
-        </is>
-      </c>
-      <c r="S231" t="inlineStr">
-        <is>
-          <t>https://ac-174auto.ru/auto/skoda/kodiaq_laurin__klement/</t>
-        </is>
-      </c>
-      <c r="T231" t="inlineStr">
-        <is>
-          <t>3058000</t>
-        </is>
-      </c>
-      <c r="U231" t="inlineStr">
-        <is>
-          <t>https://kc-klassavto.ru/auto/skoda/kodiaq_laurin__klement/</t>
-        </is>
-      </c>
       <c r="V231" t="n">
-        <v>3483600</v>
+        <v>3058000</v>
       </c>
       <c r="W231" t="inlineStr">
         <is>
@@ -13913,7 +13913,7 @@
         </is>
       </c>
       <c r="V234" t="n">
-        <v>3226800</v>
+        <v>2745000</v>
       </c>
       <c r="W234" t="inlineStr">
         <is>
@@ -13982,7 +13982,7 @@
         </is>
       </c>
       <c r="V235" t="n">
-        <v>844800</v>
+        <v>839800</v>
       </c>
       <c r="W235" t="inlineStr">
         <is>
@@ -14131,7 +14131,7 @@
         </is>
       </c>
       <c r="V238" t="n">
-        <v>425000</v>
+        <v>420000</v>
       </c>
       <c r="W238" t="inlineStr">
         <is>
@@ -14210,7 +14210,7 @@
         </is>
       </c>
       <c r="V239" t="n">
-        <v>1211000</v>
+        <v>1206000</v>
       </c>
       <c r="W239" t="inlineStr">
         <is>
@@ -14762,7 +14762,7 @@
         </is>
       </c>
       <c r="V249" t="n">
-        <v>3959400</v>
+        <v>3893000</v>
       </c>
       <c r="W249" t="inlineStr">
         <is>
@@ -15327,7 +15327,7 @@
         </is>
       </c>
       <c r="V260" t="n">
-        <v>519300</v>
+        <v>514300</v>
       </c>
       <c r="W260" t="inlineStr">
         <is>
@@ -15406,7 +15406,7 @@
         </is>
       </c>
       <c r="V261" t="n">
-        <v>1227900</v>
+        <v>1222900</v>
       </c>
       <c r="W261" t="inlineStr">
         <is>
@@ -15508,7 +15508,7 @@
         </is>
       </c>
       <c r="V263" t="n">
-        <v>2025540</v>
+        <v>1283900</v>
       </c>
       <c r="W263" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Add timeout polling, add models parser
</commit_message>
<xml_diff>
--- a/xlsx/chelyabinsk.xlsx
+++ b/xlsx/chelyabinsk.xlsx
@@ -3374,14 +3374,6 @@
           <t>https://kc-klassavto.ru/auto/faw/bestune_t55/</t>
         </is>
       </c>
-      <c r="J60" t="n">
-        <v>2064000</v>
-      </c>
-      <c r="K60" t="inlineStr">
-        <is>
-          <t>https://saturn2.ru/available-cars/faw-bestune-t55-krossover/</t>
-        </is>
-      </c>
       <c r="L60" t="inlineStr">
         <is>
           <t>1546600</t>
@@ -3451,14 +3443,6 @@
           <t>https://che-motors-2024.ru/catalog/faw/bestune_t77</t>
         </is>
       </c>
-      <c r="J61" t="n">
-        <v>2864000</v>
-      </c>
-      <c r="K61" t="inlineStr">
-        <is>
-          <t>https://saturn2.ru/available-cars/faw-bestune-t77-i-krossover/</t>
-        </is>
-      </c>
       <c r="L61" t="inlineStr">
         <is>
           <t>1918400</t>
@@ -11469,7 +11453,7 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>694</t>
+          <t>695</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
@@ -11479,30 +11463,30 @@
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>3909</t>
+          <t>3909 Бортовой грузовик</t>
         </is>
       </c>
       <c r="D224" t="n">
-        <v>1440000</v>
+        <v>1470000</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
-          <t>https://saturn2.ru/available-cars/uaz-3909/</t>
+          <t>https://saturn2.ru/available-cars/uaz-39094-bortovoy-gruzovik/</t>
         </is>
       </c>
       <c r="J224" t="n">
-        <v>1440000</v>
+        <v>1470000</v>
       </c>
       <c r="K224" t="inlineStr">
         <is>
-          <t>https://saturn2.ru/available-cars/uaz-3909/</t>
+          <t>https://saturn2.ru/available-cars/uaz-39094-bortovoy-gruzovik/</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>695</t>
+          <t>696</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
@@ -11512,30 +11496,30 @@
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>3909 Бортовой грузовик</t>
+          <t>3909 Микроавтобус</t>
         </is>
       </c>
       <c r="D225" t="n">
-        <v>1470000</v>
+        <v>1510000</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
-          <t>https://saturn2.ru/available-cars/uaz-39094-bortovoy-gruzovik/</t>
+          <t>https://saturn2.ru/available-cars/uaz-3909-mikroavtobus/</t>
         </is>
       </c>
       <c r="J225" t="n">
-        <v>1470000</v>
+        <v>1510000</v>
       </c>
       <c r="K225" t="inlineStr">
         <is>
-          <t>https://saturn2.ru/available-cars/uaz-39094-bortovoy-gruzovik/</t>
+          <t>https://saturn2.ru/available-cars/uaz-3909-mikroavtobus/</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>696</t>
+          <t>697</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
@@ -11545,30 +11529,30 @@
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>3909 Микроавтобус</t>
+          <t>3909 Скорая помощь</t>
         </is>
       </c>
       <c r="D226" t="n">
-        <v>1510000</v>
+        <v>1475000</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
-          <t>https://saturn2.ru/available-cars/uaz-3909-mikroavtobus/</t>
+          <t>https://saturn2.ru/available-cars/uaz-3909-skoraya-pomoshch/</t>
         </is>
       </c>
       <c r="J226" t="n">
-        <v>1510000</v>
+        <v>1475000</v>
       </c>
       <c r="K226" t="inlineStr">
         <is>
-          <t>https://saturn2.ru/available-cars/uaz-3909-mikroavtobus/</t>
+          <t>https://saturn2.ru/available-cars/uaz-3909-skoraya-pomoshch/</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>697</t>
+          <t>698</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
@@ -11578,30 +11562,30 @@
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>3909 Скорая помощь</t>
+          <t>3909 Цельнометаллический фургон</t>
         </is>
       </c>
       <c r="D227" t="n">
-        <v>1475000</v>
+        <v>1350000</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
-          <t>https://saturn2.ru/available-cars/uaz-3909-skoraya-pomoshch/</t>
+          <t>https://saturn2.ru/available-cars/uaz-3909-tselnometallicheskiy-furgon/</t>
         </is>
       </c>
       <c r="J227" t="n">
-        <v>1475000</v>
+        <v>1350000</v>
       </c>
       <c r="K227" t="inlineStr">
         <is>
-          <t>https://saturn2.ru/available-cars/uaz-3909-skoraya-pomoshch/</t>
+          <t>https://saturn2.ru/available-cars/uaz-3909-tselnometallicheskiy-furgon/</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>698</t>
+          <t>633</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
@@ -11611,30 +11595,38 @@
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>3909 Цельнометаллический фургон</t>
+          <t>Hunter</t>
         </is>
       </c>
       <c r="D228" t="n">
-        <v>1350000</v>
+        <v>538000</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
-          <t>https://saturn2.ru/available-cars/uaz-3909-tselnometallicheskiy-furgon/</t>
-        </is>
-      </c>
-      <c r="J228" t="n">
-        <v>1350000</v>
-      </c>
-      <c r="K228" t="inlineStr">
-        <is>
-          <t>https://saturn2.ru/available-cars/uaz-3909-tselnometallicheskiy-furgon/</t>
+          <t>https://che-motors-2024.ru/catalog/uaz/hunter</t>
+        </is>
+      </c>
+      <c r="F228" t="n">
+        <v>538000</v>
+      </c>
+      <c r="G228" t="inlineStr">
+        <is>
+          <t>https://avto-graf-newcars.ru/catalog/uaz/hunter</t>
+        </is>
+      </c>
+      <c r="H228" t="n">
+        <v>538000</v>
+      </c>
+      <c r="I228" t="inlineStr">
+        <is>
+          <t>https://che-motors-2024.ru/catalog/uaz/hunter</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>633</t>
+          <t>634</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
@@ -11644,38 +11636,56 @@
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>Hunter</t>
+          <t>Patriot</t>
         </is>
       </c>
       <c r="D229" t="n">
-        <v>538000</v>
+        <v>429380</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
-          <t>https://che-motors-2024.ru/catalog/uaz/hunter</t>
+          <t>https://che-motors-2024.ru/catalog/uaz/Patriot_2019</t>
         </is>
       </c>
       <c r="F229" t="n">
-        <v>538000</v>
+        <v>429380</v>
       </c>
       <c r="G229" t="inlineStr">
         <is>
-          <t>https://avto-graf-newcars.ru/catalog/uaz/hunter</t>
+          <t>https://avto-graf-newcars.ru/catalog/uaz/Patriot_2019</t>
         </is>
       </c>
       <c r="H229" t="n">
-        <v>538000</v>
+        <v>429380</v>
       </c>
       <c r="I229" t="inlineStr">
         <is>
-          <t>https://che-motors-2024.ru/catalog/uaz/hunter</t>
+          <t>https://che-motors-2024.ru/catalog/uaz/Patriot_2019</t>
+        </is>
+      </c>
+      <c r="L229" t="inlineStr">
+        <is>
+          <t>1108000</t>
+        </is>
+      </c>
+      <c r="M229" t="inlineStr">
+        <is>
+          <t>https://kcelitauto.ru/auto/uaz/patriot/</t>
+        </is>
+      </c>
+      <c r="P229" t="n">
+        <v>1108000</v>
+      </c>
+      <c r="Q229" t="inlineStr">
+        <is>
+          <t>https://carsklad-174.ru/auto/uaz/patriot/1rest-3/suv-5d</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>634</t>
+          <t>635</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
@@ -11685,56 +11695,30 @@
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>Patriot</t>
+          <t>Patriot New</t>
         </is>
       </c>
       <c r="D230" t="n">
-        <v>429380</v>
+        <v>1517000</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
-          <t>https://che-motors-2024.ru/catalog/uaz/Patriot_2019</t>
-        </is>
-      </c>
-      <c r="F230" t="n">
-        <v>429380</v>
-      </c>
-      <c r="G230" t="inlineStr">
-        <is>
-          <t>https://avto-graf-newcars.ru/catalog/uaz/Patriot_2019</t>
-        </is>
-      </c>
-      <c r="H230" t="n">
-        <v>429380</v>
-      </c>
-      <c r="I230" t="inlineStr">
-        <is>
-          <t>https://che-motors-2024.ru/catalog/uaz/Patriot_2019</t>
-        </is>
-      </c>
-      <c r="L230" t="inlineStr">
-        <is>
-          <t>1108000</t>
-        </is>
-      </c>
-      <c r="M230" t="inlineStr">
-        <is>
-          <t>https://kcelitauto.ru/auto/uaz/patriot/</t>
-        </is>
-      </c>
-      <c r="P230" t="n">
-        <v>1108000</v>
-      </c>
-      <c r="Q230" t="inlineStr">
-        <is>
-          <t>https://carsklad-174.ru/auto/uaz/patriot/1rest-3/suv-5d</t>
+          <t>https://saturn2.ru/available-cars/uaz-patriot-i-restayling-3-krossover/</t>
+        </is>
+      </c>
+      <c r="J230" t="n">
+        <v>1517000</v>
+      </c>
+      <c r="K230" t="inlineStr">
+        <is>
+          <t>https://saturn2.ru/available-cars/uaz-patriot-i-restayling-3-krossover/</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>635</t>
+          <t>636</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
@@ -11744,30 +11728,40 @@
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>Patriot New</t>
+          <t>Patriot Pickup</t>
         </is>
       </c>
       <c r="D231" t="n">
-        <v>1517000</v>
+        <v>1223000</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
-          <t>https://saturn2.ru/available-cars/uaz-patriot-i-restayling-3-krossover/</t>
-        </is>
-      </c>
-      <c r="J231" t="n">
-        <v>1517000</v>
-      </c>
-      <c r="K231" t="inlineStr">
-        <is>
-          <t>https://saturn2.ru/available-cars/uaz-patriot-i-restayling-3-krossover/</t>
+          <t>https://carsklad-174.ru/auto/uaz/patriot/1rest-3/pickup</t>
+        </is>
+      </c>
+      <c r="L231" t="inlineStr">
+        <is>
+          <t>1223000</t>
+        </is>
+      </c>
+      <c r="M231" t="inlineStr">
+        <is>
+          <t>https://kcelitauto.ru/auto/uaz/patriot_pickup/</t>
+        </is>
+      </c>
+      <c r="P231" t="n">
+        <v>1223000</v>
+      </c>
+      <c r="Q231" t="inlineStr">
+        <is>
+          <t>https://carsklad-174.ru/auto/uaz/patriot/1rest-3/pickup</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>636</t>
+          <t>637</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
@@ -11777,40 +11771,38 @@
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>Patriot Pickup</t>
+          <t>Pickup</t>
         </is>
       </c>
       <c r="D232" t="n">
-        <v>1223000</v>
+        <v>621000</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
-          <t>https://carsklad-174.ru/auto/uaz/patriot/1rest-3/pickup</t>
-        </is>
-      </c>
-      <c r="L232" t="inlineStr">
-        <is>
-          <t>1223000</t>
-        </is>
-      </c>
-      <c r="M232" t="inlineStr">
-        <is>
-          <t>https://kcelitauto.ru/auto/uaz/patriot_pickup/</t>
-        </is>
-      </c>
-      <c r="P232" t="n">
-        <v>1223000</v>
-      </c>
-      <c r="Q232" t="inlineStr">
-        <is>
-          <t>https://carsklad-174.ru/auto/uaz/patriot/1rest-3/pickup</t>
+          <t>https://che-motors-2024.ru/catalog/uaz/pickup-2019</t>
+        </is>
+      </c>
+      <c r="F232" t="n">
+        <v>621000</v>
+      </c>
+      <c r="G232" t="inlineStr">
+        <is>
+          <t>https://avto-graf-newcars.ru/catalog/uaz/pickup-2019</t>
+        </is>
+      </c>
+      <c r="H232" t="n">
+        <v>621000</v>
+      </c>
+      <c r="I232" t="inlineStr">
+        <is>
+          <t>https://che-motors-2024.ru/catalog/uaz/pickup-2019</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>637</t>
+          <t>638</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
@@ -11820,31 +11812,23 @@
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>Pickup</t>
+          <t>Pickup New</t>
         </is>
       </c>
       <c r="D233" t="n">
-        <v>621000</v>
+        <v>1722000</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
-          <t>https://che-motors-2024.ru/catalog/uaz/pickup-2019</t>
-        </is>
-      </c>
-      <c r="F233" t="n">
-        <v>621000</v>
-      </c>
-      <c r="G233" t="inlineStr">
-        <is>
-          <t>https://avto-graf-newcars.ru/catalog/uaz/pickup-2019</t>
-        </is>
-      </c>
-      <c r="H233" t="n">
-        <v>621000</v>
-      </c>
-      <c r="I233" t="inlineStr">
-        <is>
-          <t>https://che-motors-2024.ru/catalog/uaz/pickup-2019</t>
+          <t>https://saturn2.ru/available-cars/uaz-pickup-i-restayling-2/</t>
+        </is>
+      </c>
+      <c r="J233" t="n">
+        <v>1722000</v>
+      </c>
+      <c r="K233" t="inlineStr">
+        <is>
+          <t>https://saturn2.ru/available-cars/uaz-pickup-i-restayling-2/</t>
         </is>
       </c>
     </row>

</xml_diff>